<commit_message>
area chcek and specs files update
</commit_message>
<xml_diff>
--- a/pearson_tables/t2m_netherlands-1-1.xlsx
+++ b/pearson_tables/t2m_netherlands-1-1.xlsx
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6215684484487274</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7466287759307578</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.7818640055096155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.8294075450901187</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6704808188486789</v>
+        <v>-0.6957261489311483</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6740358687467718</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7935160894790917</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7423747362508941</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6967222522194466</v>
+        <v>0.7224527893482308</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7063499779122363</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.5896553041220011</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.7241583836993049</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -521,13 +521,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8005483505928095</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.6059289307468636</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6554702640759575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -537,13 +537,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6410823544145394</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6865716850758143</v>
+        <v>0.6337924286983915</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5996863028582465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -553,13 +553,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.6640690227375254</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.6760501457564724</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7226769569608571</v>
+        <v>0.6691467249518893</v>
       </c>
     </row>
     <row r="9">
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7351510954893362</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6140198830070225</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6927990148932234</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>